<commit_message>
Add N&C program and assets, remove old file
Added new N&C.BNR program and NNC.PNG asset. Removed outdated Naughts & Crosses.BNR file. Updated Minecraft-Computer-Operations.xlsx with related changes.
</commit_message>
<xml_diff>
--- a/Minecraft-Computer-Operations.xlsx
+++ b/Minecraft-Computer-Operations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaiha\OneDrive\Documents\GitHub\Binari-n-Rhesymegol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6C944B-BB0A-4B45-8FE9-167F5E74235C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4209312-DAF0-4BD0-8F1B-7BA6E12A8D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7613BB6-1CB0-4729-A24E-D1ACFF1E0467}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{B7613BB6-1CB0-4729-A24E-D1ACFF1E0467}"/>
   </bookViews>
   <sheets>
     <sheet name="Operation Mapping" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t>OP CODE</t>
   </si>
@@ -279,6 +279,21 @@
   </si>
   <si>
     <t>MORE MEMS</t>
+  </si>
+  <si>
+    <t>CLSOU</t>
+  </si>
+  <si>
+    <t>CLEAR SPESH</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>USERIN</t>
+  </si>
+  <si>
+    <t>BŴTIN</t>
   </si>
 </sst>
 </file>
@@ -365,25 +380,25 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,30 +740,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4783DD8-DB99-4203-8706-5C5B54F85F4F}">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
       <c r="J1" s="2" t="str">
         <f>DEC2BIN(A3,3)</f>
         <v>001</v>
@@ -777,34 +792,34 @@
         <f>DEC2BIN(A9,3)</f>
         <v>111</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="str">
+      <c r="B2" s="9"/>
+      <c r="C2" s="8" t="str">
         <f>DEC2BIN(A2,5)</f>
         <v>00000</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -812,32 +827,32 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="str">
+      <c r="B3" s="9"/>
+      <c r="C3" s="8" t="str">
         <f t="shared" ref="C3:C33" si="0">DEC2BIN(A3,5)</f>
         <v>00001</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -845,34 +860,34 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="str">
+      <c r="B4" s="9"/>
+      <c r="C4" s="8" t="str">
         <f t="shared" si="0"/>
         <v>00010</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -880,34 +895,34 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="str">
+      <c r="B5" s="9"/>
+      <c r="C5" s="8" t="str">
         <f>DEC2BIN(A5,5)</f>
         <v>00011</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -915,34 +930,34 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="str">
+      <c r="B6" s="9"/>
+      <c r="C6" s="8" t="str">
         <f t="shared" si="0"/>
         <v>00100</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -950,100 +965,100 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="7" t="s">
+      <c r="Q6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6" t="str">
+      <c r="B7" s="9"/>
+      <c r="C7" s="8" t="str">
         <f t="shared" si="0"/>
         <v>00101</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6" t="str">
+      <c r="B8" s="9"/>
+      <c r="C8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>00110</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="9">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6" t="str">
+      <c r="B9" s="9"/>
+      <c r="C9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>00111</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1065,32 +1080,32 @@
       <c r="P9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6" t="str">
+      <c r="B10" s="9"/>
+      <c r="C10" s="8" t="str">
         <f t="shared" si="0"/>
         <v>01000</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
       <c r="J10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1108,32 +1123,32 @@
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="9">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6" t="str">
+      <c r="B11" s="9"/>
+      <c r="C11" s="8" t="str">
         <f t="shared" si="0"/>
         <v>01001</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="8"/>
+      <c r="E11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
       <c r="J11" s="2" t="s">
         <v>73</v>
       </c>
@@ -1155,32 +1170,32 @@
       <c r="P11" s="2">
         <v>7</v>
       </c>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6" t="str">
+      <c r="B12" s="9"/>
+      <c r="C12" s="8" t="str">
         <f t="shared" si="0"/>
         <v>01010</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="3" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
       <c r="J12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1192,34 +1207,34 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
-      <c r="Q12" s="7" t="s">
+      <c r="Q12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="str">
+      <c r="B13" s="9"/>
+      <c r="C13" s="8" t="str">
         <f t="shared" si="0"/>
         <v>01011</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="7"/>
+      <c r="G13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1227,32 +1242,32 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6" t="str">
+      <c r="B14" s="9"/>
+      <c r="C14" s="8" t="str">
         <f t="shared" si="0"/>
         <v>01100</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="8"/>
+      <c r="E14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="7"/>
+      <c r="G14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="2" t="s">
         <v>33</v>
       </c>
@@ -1268,32 +1283,32 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="str">
+      <c r="B15" s="9"/>
+      <c r="C15" s="8" t="str">
         <f t="shared" si="0"/>
         <v>01101</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3" t="s">
+      <c r="F15" s="7"/>
+      <c r="G15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1301,32 +1316,32 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="9">
         <v>14</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6" t="str">
+      <c r="B16" s="9"/>
+      <c r="C16" s="8" t="str">
         <f t="shared" si="0"/>
         <v>01110</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="3" t="s">
+      <c r="F16" s="7"/>
+      <c r="G16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1334,32 +1349,32 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6" t="str">
+      <c r="B17" s="9"/>
+      <c r="C17" s="8" t="str">
         <f t="shared" si="0"/>
         <v>01111</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="8"/>
+      <c r="E17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="3" t="s">
+      <c r="F17" s="7"/>
+      <c r="G17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
       <c r="J17" s="2">
         <v>1</v>
       </c>
@@ -1381,32 +1396,32 @@
       <c r="P17" s="2">
         <v>7</v>
       </c>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6" t="str">
+      <c r="B18" s="9"/>
+      <c r="C18" s="8" t="str">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3" t="s">
+      <c r="F18" s="7"/>
+      <c r="G18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
       <c r="J18" s="2" t="s">
         <v>35</v>
       </c>
@@ -1424,32 +1439,32 @@
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="9">
         <v>17</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6" t="str">
+      <c r="B19" s="9"/>
+      <c r="C19" s="8" t="str">
         <f t="shared" si="0"/>
         <v>10001</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4" t="s">
+      <c r="D19" s="8"/>
+      <c r="E19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="3" t="s">
+      <c r="F19" s="7"/>
+      <c r="G19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1457,32 +1472,32 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="9">
         <v>18</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6" t="str">
+      <c r="B20" s="9"/>
+      <c r="C20" s="8" t="str">
         <f t="shared" si="0"/>
         <v>10010</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="4" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="3" t="s">
+      <c r="F20" s="7"/>
+      <c r="G20" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1490,32 +1505,32 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="9">
         <v>19</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6" t="str">
+      <c r="B21" s="9"/>
+      <c r="C21" s="8" t="str">
         <f t="shared" si="0"/>
         <v>10011</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="8"/>
+      <c r="E21" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="3" t="s">
+      <c r="F21" s="7"/>
+      <c r="G21" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
       <c r="J21" s="2" t="s">
         <v>79</v>
       </c>
@@ -1527,28 +1542,28 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="9">
         <v>20</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6" t="str">
+      <c r="B22" s="9"/>
+      <c r="C22" s="8" t="str">
         <f t="shared" si="0"/>
         <v>10100</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -1556,28 +1571,28 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="9">
         <v>21</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6" t="str">
+      <c r="B23" s="9"/>
+      <c r="C23" s="8" t="str">
         <f t="shared" si="0"/>
         <v>10101</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -1585,28 +1600,28 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="9">
         <v>22</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6" t="str">
+      <c r="B24" s="9"/>
+      <c r="C24" s="8" t="str">
         <f t="shared" si="0"/>
         <v>10110</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="8"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -1614,28 +1629,28 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="9">
         <v>23</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6" t="str">
+      <c r="B25" s="9"/>
+      <c r="C25" s="8" t="str">
         <f t="shared" si="0"/>
         <v>10111</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -1643,61 +1658,71 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7"/>
-      <c r="U25" s="7"/>
-      <c r="V25" s="7"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="9">
         <v>24</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6" t="str">
+      <c r="B26" s="9"/>
+      <c r="C26" s="8" t="str">
         <f t="shared" si="0"/>
         <v>11000</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
-      <c r="U26" s="7"/>
-      <c r="V26" s="7"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="9">
         <v>25</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6" t="str">
+      <c r="B27" s="9"/>
+      <c r="C27" s="8" t="str">
         <f t="shared" si="0"/>
         <v>11001</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="4" t="s">
+      <c r="D27" s="8"/>
+      <c r="E27" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="3" t="s">
+      <c r="F27" s="7"/>
+      <c r="G27" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -1705,32 +1730,32 @@
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="9">
         <v>26</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="6" t="str">
+      <c r="B28" s="9"/>
+      <c r="C28" s="8" t="str">
         <f t="shared" si="0"/>
         <v>11010</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="4" t="s">
+      <c r="D28" s="8"/>
+      <c r="E28" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="3" t="s">
+      <c r="F28" s="7"/>
+      <c r="G28" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -1738,32 +1763,32 @@
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="9">
         <v>27</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="6" t="str">
+      <c r="B29" s="9"/>
+      <c r="C29" s="8" t="str">
         <f t="shared" si="0"/>
         <v>11011</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="4" t="s">
+      <c r="D29" s="8"/>
+      <c r="E29" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="3" t="s">
+      <c r="F29" s="7"/>
+      <c r="G29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -1771,32 +1796,32 @@
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="9">
         <v>28</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6" t="str">
+      <c r="B30" s="9"/>
+      <c r="C30" s="8" t="str">
         <f t="shared" si="0"/>
         <v>11100</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="4" t="s">
+      <c r="D30" s="8"/>
+      <c r="E30" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="3" t="s">
+      <c r="F30" s="7"/>
+      <c r="G30" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -1804,34 +1829,34 @@
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
-      <c r="Q30" s="7" t="s">
+      <c r="Q30" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
-      <c r="V30" s="7"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="9">
         <v>29</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="6" t="str">
+      <c r="B31" s="9"/>
+      <c r="C31" s="8" t="str">
         <f t="shared" si="0"/>
         <v>11101</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="4" t="s">
+      <c r="D31" s="8"/>
+      <c r="E31" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="3" t="s">
+      <c r="F31" s="7"/>
+      <c r="G31" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
       <c r="J31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1847,83 +1872,226 @@
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
-      <c r="Q31" s="7" t="s">
+      <c r="Q31" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="6" t="str">
+      <c r="B32" s="9"/>
+      <c r="C32" s="8" t="str">
         <f t="shared" si="0"/>
         <v>11110</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="4" t="s">
+      <c r="D32" s="8"/>
+      <c r="E32" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="3" t="s">
+      <c r="F32" s="7"/>
+      <c r="G32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="A33" s="9">
         <v>31</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="6" t="str">
+      <c r="B33" s="9"/>
+      <c r="C33" s="8" t="str">
         <f t="shared" si="0"/>
         <v>11111</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="4" t="s">
+      <c r="D33" s="8"/>
+      <c r="E33" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="3" t="s">
+      <c r="F33" s="7"/>
+      <c r="G33" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="7"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="167">
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="Q14:V14"/>
+    <mergeCell ref="Q15:V15"/>
+    <mergeCell ref="Q16:V16"/>
+    <mergeCell ref="Q17:V17"/>
+    <mergeCell ref="Q18:V18"/>
+    <mergeCell ref="Q11:V11"/>
+    <mergeCell ref="Q19:V19"/>
+    <mergeCell ref="Q2:V2"/>
+    <mergeCell ref="Q3:V3"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="Q5:V5"/>
+    <mergeCell ref="Q6:V6"/>
+    <mergeCell ref="Q7:V7"/>
+    <mergeCell ref="Q8:V8"/>
+    <mergeCell ref="Q9:V9"/>
+    <mergeCell ref="Q10:V10"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E12:F12"/>
     <mergeCell ref="J32:P32"/>
     <mergeCell ref="J33:P33"/>
     <mergeCell ref="G7:I7"/>
@@ -1948,149 +2116,6 @@
     <mergeCell ref="Q28:V28"/>
     <mergeCell ref="Q12:V12"/>
     <mergeCell ref="Q13:V13"/>
-    <mergeCell ref="Q10:V10"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="Q14:V14"/>
-    <mergeCell ref="Q15:V15"/>
-    <mergeCell ref="Q16:V16"/>
-    <mergeCell ref="Q17:V17"/>
-    <mergeCell ref="Q18:V18"/>
-    <mergeCell ref="Q11:V11"/>
-    <mergeCell ref="Q19:V19"/>
-    <mergeCell ref="Q2:V2"/>
-    <mergeCell ref="Q3:V3"/>
-    <mergeCell ref="Q4:V4"/>
-    <mergeCell ref="Q5:V5"/>
-    <mergeCell ref="Q6:V6"/>
-    <mergeCell ref="Q7:V7"/>
-    <mergeCell ref="Q8:V8"/>
-    <mergeCell ref="Q9:V9"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>